<commit_message>
ADC working with DMA
</commit_message>
<xml_diff>
--- a/doc/robo.xlsx
+++ b/doc/robo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\robot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EB244-A1B6-4141-922F-4AEBD10B35A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02043161-3811-472F-99C1-F06C7759C675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0931673-A5ED-4057-83E7-7902F2F65021}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>STM32</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>Motor1_EN</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>ADC[0]</t>
+  </si>
+  <si>
+    <t>ADC[1]</t>
+  </si>
+  <si>
+    <t>ADC[2]</t>
   </si>
 </sst>
 </file>
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C140F1C-262D-48F9-B43F-294F3E62814A}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +594,7 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,52 +602,67 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -643,7 +670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -651,12 +678,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -664,7 +691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -672,7 +699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -680,7 +707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -688,12 +715,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Remove DMA - ADC working in injected mode
</commit_message>
<xml_diff>
--- a/doc/robo.xlsx
+++ b/doc/robo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\robot\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Porath\git\robot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02043161-3811-472F-99C1-F06C7759C675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B0A675-1F1F-4510-B762-357FC17EAA09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0931673-A5ED-4057-83E7-7902F2F65021}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0931673-A5ED-4057-83E7-7902F2F65021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -585,16 +585,16 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,12 +602,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -618,7 +618,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -629,7 +629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -640,7 +640,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -651,7 +651,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -662,7 +662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -670,7 +670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -678,12 +678,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -691,7 +691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -699,7 +699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -707,7 +707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -715,17 +715,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -733,12 +733,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -746,7 +746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -754,7 +754,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -762,17 +762,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -780,7 +780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -788,17 +788,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -806,7 +806,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -814,7 +814,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -822,7 +822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -830,7 +830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -838,12 +838,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -851,7 +851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -859,7 +859,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>

</xml_diff>